<commit_message>
TMBA now using tech mapping
</commit_message>
<xml_diff>
--- a/mat_dp_pipeline/data_sources/Technology_Codes.xlsx
+++ b/mat_dp_pipeline/data_sources/Technology_Codes.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$2:$D$80</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$2:$E$80</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="233">
   <si>
     <t xml:space="preserve">Technologies</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
     <t xml:space="preserve">tech_grl</t>
   </si>
   <si>
@@ -163,6 +166,9 @@
     <t xml:space="preserve">Biomass Power Plant</t>
   </si>
   <si>
+    <t xml:space="preserve">Power plant</t>
+  </si>
+  <si>
     <t xml:space="preserve">Biomass</t>
   </si>
   <si>
@@ -716,9 +722,6 @@
   </si>
   <si>
     <t xml:space="preserve">PHEV_avg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">power_trade</t>
   </si>
 </sst>
 </file>
@@ -1048,22 +1051,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="21.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="43.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="17.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="21.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="43.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1071,6 +1074,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -1079,13 +1083,13 @@
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="0" t="s">
@@ -1100,1122 +1104,1270 @@
       <c r="I2" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="J2" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>17</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>19</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>21</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>23</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>25</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>27</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>29</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>31</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>33</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>35</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>37</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>39</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>41</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>43</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="0" t="s">
         <v>46</v>
       </c>
+      <c r="C20" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="D20" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G20" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" s="7"/>
+      <c r="J20" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="H20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="I21" s="8" t="s">
         <v>55</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G22" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="J22" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="I22" s="7"/>
-    </row>
-    <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I23" s="8" t="s">
         <v>67</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="I24" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G25" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="J25" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="I25" s="7"/>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="G26" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="H26" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G27" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="J27" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="I27" s="7"/>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="G28" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="H28" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="C28" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="I28" s="7"/>
-    </row>
-    <row r="29" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J28" s="7"/>
+    </row>
+    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="I29" s="8" t="s">
         <v>92</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>97</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="I30" s="7"/>
+        <v>99</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="G31" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="H31" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="C31" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="G31" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="I31" s="7"/>
+      <c r="J31" s="0" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B32" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="C32" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>101</v>
-      </c>
       <c r="E32" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="I32" s="7"/>
+        <v>99</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="J32" s="7"/>
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="I33" s="7"/>
+        <v>108</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="J33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="I34" s="8" t="s">
-        <v>110</v>
+        <v>112</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="I35" s="7"/>
+        <v>116</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="J35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>119</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="I36" s="7"/>
+        <v>121</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="J36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="I37" s="8" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H37" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="H38" s="7"/>
-    </row>
-    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>131</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="I38" s="7"/>
+      <c r="J38" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="H39" s="7"/>
-    </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>134</v>
+      </c>
+      <c r="C39" s="6"/>
+      <c r="I39" s="7"/>
+    </row>
+    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="H40" s="7"/>
-    </row>
-    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>136</v>
+      </c>
+      <c r="C40" s="6"/>
+      <c r="I40" s="7"/>
+    </row>
+    <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="H41" s="7"/>
-    </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>138</v>
+      </c>
+      <c r="C41" s="6"/>
+      <c r="I41" s="7"/>
+    </row>
+    <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>140</v>
+      </c>
+      <c r="C42" s="6"/>
+    </row>
+    <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>74</v>
+        <v>142</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>77</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>95</v>
+        <v>144</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F44" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="H44" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="G44" s="0" t="s">
+      <c r="E45" s="0" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="F45" s="7" t="s">
+      <c r="F45" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H45" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C46" s="6"/>
+    </row>
+    <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C47" s="6"/>
+    </row>
+    <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C48" s="6"/>
+    </row>
+    <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C49" s="6"/>
+    </row>
+    <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C50" s="6"/>
+    </row>
+    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C51" s="6"/>
+    </row>
+    <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C52" s="6"/>
+    </row>
+    <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C53" s="6"/>
+    </row>
+    <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C54" s="6"/>
+    </row>
+    <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C55" s="6"/>
+    </row>
+    <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C56" s="6"/>
+    </row>
+    <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C57" s="6"/>
+    </row>
+    <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C58" s="6"/>
+    </row>
+    <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C59" s="6"/>
+    </row>
+    <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C60" s="6"/>
+    </row>
+    <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C61" s="6"/>
+    </row>
+    <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C62" s="6"/>
+    </row>
+    <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C63" s="6"/>
+    </row>
+    <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C64" s="6"/>
+    </row>
+    <row r="65" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C65" s="6"/>
+    </row>
+    <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C66" s="6"/>
+    </row>
+    <row r="67" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C67" s="6"/>
+    </row>
+    <row r="68" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="C68" s="6"/>
+    </row>
+    <row r="69" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C69" s="6"/>
+    </row>
+    <row r="70" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="C70" s="6"/>
+    </row>
+    <row r="71" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="C71" s="6"/>
+    </row>
+    <row r="72" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="C72" s="6"/>
+    </row>
+    <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="C73" s="6"/>
+    </row>
+    <row r="74" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C74" s="6"/>
+    </row>
+    <row r="75" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C75" s="6"/>
+    </row>
+    <row r="76" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C76" s="10"/>
+    </row>
+    <row r="77" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="B77" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="C77" s="12"/>
+    </row>
+    <row r="78" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="B78" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="E78" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F78" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="B79" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D79" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="G45" s="0" t="s">
+      <c r="E79" s="0" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="B74" s="6" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="B76" s="10" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="B77" s="12" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="B78" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="C78" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="D78" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="E78" s="0" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="B79" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="C79" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="D79" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="E79" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="F79" s="7" t="s">
+      <c r="F79" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="G79" s="0" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G79" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H79" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="13" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>214</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>117</v>
+        <v>216</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F80" s="0" t="s">
         <v>119</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F81" s="0" t="s">
-        <v>215</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="H80" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G81" s="0" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C82" s="0" t="s">
         <v>217</v>
       </c>
+      <c r="H81" s="0" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C82" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="D82" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C83" s="0" t="s">
         <v>221</v>
       </c>
+      <c r="H82" s="0" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D83" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>221</v>
-      </c>
-      <c r="H83" s="0" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C84" s="0" t="s">
         <v>223</v>
       </c>
+      <c r="F83" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="I83" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D84" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="H84" s="0" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C85" s="0" t="s">
         <v>225</v>
       </c>
+      <c r="F84" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="I84" s="0" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D85" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="H85" s="0" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C86" s="0" t="s">
         <v>227</v>
       </c>
+      <c r="F85" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="I85" s="0" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D86" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="H86" s="0" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C87" s="0" t="s">
         <v>229</v>
       </c>
+      <c r="F86" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="I86" s="0" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D87" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="H87" s="0" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I88" s="8" t="s">
         <v>231</v>
       </c>
-    </row>
+      <c r="F87" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="I87" s="0" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A2:D80"/>
+  <autoFilter ref="A2:E80"/>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Integrated Assesment Model data source
</commit_message>
<xml_diff>
--- a/mat_dp_pipeline/data_sources/Technology_Codes.xlsx
+++ b/mat_dp_pipeline/data_sources/Technology_Codes.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="218">
   <si>
     <t xml:space="preserve">Technologies</t>
   </si>
@@ -175,9 +175,6 @@
     <t xml:space="preserve">Biomass|w/o CCS</t>
   </si>
   <si>
-    <t xml:space="preserve">Capacity Additions|Electricity|Biomass|w/o CCS</t>
-  </si>
-  <si>
     <t xml:space="preserve">PWRBIO00C</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
     <t xml:space="preserve">Biomass|w/ CCS</t>
   </si>
   <si>
-    <t xml:space="preserve">Capacity Additions|Electricity|Biomass|w/ CCS</t>
-  </si>
-  <si>
     <t xml:space="preserve">Biomass with ccs</t>
   </si>
   <si>
@@ -211,9 +205,6 @@
     <t xml:space="preserve">Coal|w/o CCS</t>
   </si>
   <si>
-    <t xml:space="preserve">Capacity Additions|Electricity|Coal|w/o CCS</t>
-  </si>
-  <si>
     <t xml:space="preserve">PWRCOA00C</t>
   </si>
   <si>
@@ -229,9 +220,6 @@
     <t xml:space="preserve">Coal|w/ CCS</t>
   </si>
   <si>
-    <t xml:space="preserve">Capacity Additions|Electricity|Coal|w/ CCS</t>
-  </si>
-  <si>
     <t xml:space="preserve">Coal with ccs</t>
   </si>
   <si>
@@ -244,9 +232,6 @@
     <t xml:space="preserve">Geothermal</t>
   </si>
   <si>
-    <t xml:space="preserve">Capacity Additions|Electricity|Geothermal</t>
-  </si>
-  <si>
     <t xml:space="preserve">PWROHC001</t>
   </si>
   <si>
@@ -259,9 +244,6 @@
     <t xml:space="preserve">Oil|w/o CCS</t>
   </si>
   <si>
-    <t xml:space="preserve">Capacity Additions|Electricity|Oil|w/o CCS</t>
-  </si>
-  <si>
     <t xml:space="preserve">PWROHC002</t>
   </si>
   <si>
@@ -280,9 +262,6 @@
     <t xml:space="preserve">Gas|w/o CCS</t>
   </si>
   <si>
-    <t xml:space="preserve">Capacity Additions|Electricity|Gas|w/o CCS</t>
-  </si>
-  <si>
     <t xml:space="preserve">PWRNGS002</t>
   </si>
   <si>
@@ -304,9 +283,6 @@
     <t xml:space="preserve">Gas|w/ CCS</t>
   </si>
   <si>
-    <t xml:space="preserve">Capacity Additions|Electricity|Gas|w/ CCS</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gas with ccs</t>
   </si>
   <si>
@@ -325,9 +301,6 @@
     <t xml:space="preserve">Solar</t>
   </si>
   <si>
-    <t xml:space="preserve">Capacity Additions|Electricity|Solar</t>
-  </si>
-  <si>
     <t xml:space="preserve">PWRCSP001</t>
   </si>
   <si>
@@ -364,9 +337,6 @@
     <t xml:space="preserve">Hydro</t>
   </si>
   <si>
-    <t xml:space="preserve">Capacity Additions|Electricity|Hydro</t>
-  </si>
-  <si>
     <t xml:space="preserve">PWRHYD003</t>
   </si>
   <si>
@@ -391,9 +361,6 @@
     <t xml:space="preserve">Wind|Onshore</t>
   </si>
   <si>
-    <t xml:space="preserve">Capacity Additions|Electricity|Wind|Onshore</t>
-  </si>
-  <si>
     <t xml:space="preserve">PWRWND002</t>
   </si>
   <si>
@@ -406,9 +373,6 @@
     <t xml:space="preserve">Wind|Offshore</t>
   </si>
   <si>
-    <t xml:space="preserve">Capacity Additions|Electricity|Wind|Offshore</t>
-  </si>
-  <si>
     <t xml:space="preserve">Wind</t>
   </si>
   <si>
@@ -421,9 +385,6 @@
     <t xml:space="preserve">Nuclear</t>
   </si>
   <si>
-    <t xml:space="preserve">Capacity Additions|Electricity|Nuclear</t>
-  </si>
-  <si>
     <t xml:space="preserve">PWRTRNIMP</t>
   </si>
   <si>
@@ -679,9 +640,6 @@
     <t xml:space="preserve">Storage Capacity</t>
   </si>
   <si>
-    <t xml:space="preserve">Capacity Additions|Electricity|Storage Capacity</t>
-  </si>
-  <si>
     <t xml:space="preserve">Oil CCS</t>
   </si>
   <si>
@@ -689,9 +647,6 @@
   </si>
   <si>
     <t xml:space="preserve">Oil|w/ CCS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capacity Additions|Electricity|Oil|w/ CCS</t>
   </si>
   <si>
     <t xml:space="preserve">BEV medium car</t>
@@ -1051,10 +1006,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J1048576"/>
+  <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F82" activeCellId="0" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1069,14 +1024,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.15"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1284,7 +1239,7 @@
         <v>49</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="0" t="s">
@@ -1293,986 +1248,986 @@
     </row>
     <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="C21" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="0" t="s">
+      <c r="E21" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="F21" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="H21" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="G21" s="0" t="s">
+      <c r="J21" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="E22" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="G22" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>61</v>
-      </c>
       <c r="H22" s="0" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="F23" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="0" t="s">
+      <c r="H23" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="J23" s="8" t="s">
         <v>65</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="J23" s="8" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="J26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="J28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="J32" s="7"/>
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="J33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="J34" s="8" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="J35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="J36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="J37" s="8" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="I38" s="7"/>
       <c r="J38" s="0" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="C39" s="6"/>
       <c r="I39" s="7"/>
     </row>
     <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="C40" s="6"/>
       <c r="I40" s="7"/>
     </row>
     <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="C41" s="6"/>
       <c r="I41" s="7"/>
     </row>
     <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="C42" s="6"/>
     </row>
     <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="C46" s="6"/>
     </row>
     <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="C47" s="6"/>
     </row>
     <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="C48" s="6"/>
     </row>
     <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="C49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="C50" s="6"/>
     </row>
     <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="C51" s="6"/>
     </row>
     <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="C52" s="6"/>
     </row>
     <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="C53" s="6"/>
     </row>
     <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="C54" s="6"/>
     </row>
     <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="C55" s="6"/>
     </row>
     <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="C56" s="6"/>
     </row>
     <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="C57" s="6"/>
     </row>
     <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="5" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="C58" s="6"/>
     </row>
     <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="5" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="C59" s="6"/>
     </row>
     <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="5" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="C60" s="6"/>
     </row>
     <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="5" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="C61" s="6"/>
     </row>
     <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="5" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="C62" s="6"/>
     </row>
     <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="5" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="C63" s="6"/>
     </row>
     <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="5" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C64" s="6"/>
     </row>
     <row r="65" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="5" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C65" s="6"/>
     </row>
     <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="5" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C66" s="6"/>
     </row>
     <row r="67" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="5" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="C67" s="6"/>
     </row>
     <row r="68" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="5" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="C68" s="6"/>
     </row>
     <row r="69" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="5" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="C69" s="6"/>
     </row>
     <row r="70" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="5" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="5" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="5" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="C72" s="6"/>
     </row>
     <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="5" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="C73" s="6"/>
     </row>
     <row r="74" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="5" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="C74" s="6"/>
     </row>
     <row r="75" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="5" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="C75" s="6"/>
     </row>
     <row r="76" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="9" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="C76" s="10"/>
     </row>
     <row r="77" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="11" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="C77" s="12"/>
     </row>
     <row r="78" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="11" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="13" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="G79" s="7" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="H79" s="0" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="13" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="H80" s="0" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G81" s="0" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="H81" s="0" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2280,92 +2235,88 @@
         <v>47</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="F82" s="0" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="H82" s="0" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D83" s="0" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I83" s="0" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D84" s="0" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="F84" s="0" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="I84" s="0" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D85" s="0" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="I85" s="0" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D86" s="0" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="F86" s="0" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="I86" s="0" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D87" s="0" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="F87" s="0" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="I87" s="0" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>217</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:E80"/>
   <mergeCells count="1">

</xml_diff>